<commit_message>
fix data for current situation
</commit_message>
<xml_diff>
--- a/Actigraphic Studies.xlsx
+++ b/Actigraphic Studies.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11015"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stitc\Desktop\UW\Info201\Final Project\info201agsleepdeprivation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/phuongvu/Desktop/UW/Autumn 2019/INFO 201/info201agsleepdeprivation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{552CE5ED-11A9-4E7C-B13E-7971017F2066}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1569230E-2BCA-7741-8326-A8203BAD7958}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13368" yWindow="1332" windowWidth="12192" windowHeight="9924" xr2:uid="{B370AFF0-FEC2-B04F-8E53-BAD42E22327F}"/>
+    <workbookView xWindow="13360" yWindow="1340" windowWidth="12200" windowHeight="9920" xr2:uid="{B370AFF0-FEC2-B04F-8E53-BAD42E22327F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,24 +25,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
-  <si>
-    <t>Year</t>
-  </si>
-  <si>
-    <t>Age Range</t>
-  </si>
-  <si>
-    <t>Total Sleep Time(min)</t>
-  </si>
-  <si>
-    <t>20-34</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
   <si>
     <t>22-24</t>
   </si>
   <si>
     <t>20-30</t>
+  </si>
+  <si>
+    <t>sleep_time</t>
+  </si>
+  <si>
+    <t>age_range</t>
+  </si>
+  <si>
+    <t>year</t>
   </si>
 </sst>
 </file>
@@ -394,132 +391,110 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17847C85-52BD-7049-8028-87E35887B19D}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="C3" sqref="A2:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>1996</v>
-      </c>
-      <c r="B2">
-        <v>29.95</v>
+        <v>2000</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
       </c>
       <c r="C2">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+        <v>558.70000000000005</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>1997</v>
+        <v>2000</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C3">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+        <v>511.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2000</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C4">
-        <v>558.70000000000005</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+        <v>517.70000000000005</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>2000</v>
-      </c>
-      <c r="B5" t="s">
-        <v>4</v>
+        <v>2003</v>
+      </c>
+      <c r="B5">
+        <v>35.35</v>
       </c>
       <c r="C5">
-        <v>511.5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+        <v>383.93</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>2000</v>
-      </c>
-      <c r="B6" t="s">
-        <v>4</v>
+        <v>2006</v>
+      </c>
+      <c r="B6">
+        <v>27.7</v>
       </c>
       <c r="C6">
-        <v>517.70000000000005</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>2003</v>
+        <v>2010</v>
       </c>
       <c r="B7">
-        <v>35.35</v>
+        <v>35.6</v>
       </c>
       <c r="C7">
-        <v>383.93</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>2006</v>
+        <v>2010</v>
       </c>
       <c r="B8">
-        <v>27.7</v>
+        <v>25</v>
       </c>
       <c r="C8">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+        <v>437.7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>2010</v>
-      </c>
-      <c r="B9">
-        <v>35.6</v>
+        <v>2012</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1</v>
       </c>
       <c r="C9">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>2010</v>
-      </c>
-      <c r="B10">
-        <v>25</v>
-      </c>
-      <c r="C10">
-        <v>437.7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>2012</v>
-      </c>
-      <c r="B11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11">
         <v>369</v>
       </c>
     </row>

</xml_diff>